<commit_message>
with second sheet AZ and Data Center
</commit_message>
<xml_diff>
--- a/Cloud_Intro.xlsx
+++ b/Cloud_Intro.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94665526-5CD0-43B0-8E3B-9A269A9712A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C23B2-54EE-4646-9299-9DF52AE12194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63294D6A-0B05-4D87-BEAB-6A8C9DAED151}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{63294D6A-0B05-4D87-BEAB-6A8C9DAED151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Packaged Software</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>It provides a centrally hosted and managed software services to the end users. It delivers software over the internet, on-demand nd typically follows a subscription model. Ex : Office 365, One Drive, Kindle, Dropbox etc. It is a model where operational cost is minimum.</t>
+  </si>
+  <si>
+    <t>SERVERLESS COMPUTING</t>
   </si>
 </sst>
 </file>
@@ -297,6 +301,280 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF66117-8532-93E7-3184-3AA420B9121E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="518160" y="449580"/>
+          <a:ext cx="7299960" cy="2606040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9309CF9B-D78A-325F-D9C5-5C67B01AE560}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="662940" y="312420"/>
+          <a:ext cx="7059010" cy="2943636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{401BB862-7D65-34FB-106E-284A90C54B86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8648700" y="487680"/>
+          <a:ext cx="6827520" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Each</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
+            <a:t> Availability Zone has datacenter and each data center has fault and update domains.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>191598</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7F5BCEB-017E-ACCC-76AF-26545F08F0D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="830580"/>
+          <a:ext cx="5639898" cy="2915280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A4E9CA-B63F-0D1D-120C-859EE27092EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5974080" y="1036320"/>
+          <a:ext cx="3764280" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -601,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4A69E5-D122-4F1D-9136-6558604D66F2}">
   <dimension ref="D2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,8 +892,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="E2">
-        <v>3</v>
+      <c r="E2" t="s">
+        <v>26</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -814,4 +1092,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6651D4E-6B4E-4221-9EBF-98D277F70ED4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>